<commit_message>
MALS-1134 Fix registrant name columns
</commit_message>
<xml_diff>
--- a/app/server/static/templates/reports/Apiary_Producer_Report_City_Template.xlsx
+++ b/app/server/static/templates/reports/Apiary_Producer_Report_City_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MALS\app\server\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C083E93F-8E30-46BB-9A07-EC8F968809E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8141917B-0CD8-4922-8E4C-A5A871EFBEF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
   </bookViews>
@@ -95,12 +95,6 @@
     <t>{d.Reg[i].LicenceNumber}</t>
   </si>
   <si>
-    <t>{d.Reg[i].Lastname}</t>
-  </si>
-  <si>
-    <t>{d.Reg[i].Firstname}</t>
-  </si>
-  <si>
     <t>{d.Reg[i].PrimaryPhone}</t>
   </si>
   <si>
@@ -129,6 +123,12 @@
   </si>
   <si>
     <t>Date &amp; Time Report Created (UTC)</t>
+  </si>
+  <si>
+    <t>{d.Reg[i].LastName}</t>
+  </si>
+  <si>
+    <t>{d.Reg[i].FirstName}</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +565,7 @@
       <c r="F1" s="11"/>
       <c r="H1" s="1"/>
       <c r="I1" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>14</v>
@@ -667,33 +667,33 @@
         <v>19</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="E7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="F7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="G7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="H7" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="I7" s="9" t="s">
         <v>25</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="10"/>
@@ -703,13 +703,13 @@
         <v>12</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H12" s="12" t="s">
         <v>11</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -723,12 +723,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8CBF3948AF16E4A9427EB9CB0C3AFDB" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9fc8a81a77eeb73bda9729b3f784b8c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bc8b8595-9fa1-49bc-a016-2621e7bde64e" xmlns:ns3="e1c8ebbc-f196-4c28-98e9-1900bd408e79" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="88ad40c7f0e134defa4acd5e486d3459" ns2:_="" ns3:_="">
     <xsd:import namespace="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
@@ -939,6 +933,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -949,23 +949,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AE8867F-A406-43FE-8CA7-900664EF104F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6470599-A386-4A6B-9059-1EE4DCF6BB3B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -984,6 +967,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AE8867F-A406-43FE-8CA7-900664EF104F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03155FF8-1FF1-4181-B2B9-505B2808F58D}">
   <ds:schemaRefs>

</xml_diff>